<commit_message>
Finished report & updated few other bits
</commit_message>
<xml_diff>
--- a/Test Results.xlsx
+++ b/Test Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20680" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15500" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Difficulty</t>
   </si>
   <si>
     <t>Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Attempts</t>
   </si>
 </sst>
 </file>
@@ -48,12 +54,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,8 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,6 +210,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$1:$G$1</c:f>
@@ -224,22 +258,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.00031708</c:v>
+                  <c:v>0.0002664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0015232</c:v>
+                  <c:v>0.0025323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.034209</c:v>
+                  <c:v>0.06798</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39387</c:v>
+                  <c:v>0.67805</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.01133</c:v>
+                  <c:v>11.102</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.941</c:v>
+                  <c:v>202.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -254,11 +288,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-42052928"/>
-        <c:axId val="-42057248"/>
+        <c:axId val="1433416784"/>
+        <c:axId val="1432761216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-42052928"/>
+        <c:axId val="1433416784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -334,6 +368,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -370,13 +405,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-42057248"/>
+        <c:crossAx val="1432761216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-42057248"/>
+        <c:axId val="1432761216"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -492,7 +528,478 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-42052928"/>
+        <c:crossAx val="1433416784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Attempts to Solve POW against Difficulty</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>24.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6481.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63353.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0989458E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.18380634E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1454559168"/>
+        <c:axId val="1456304576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1454559168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Difficulty</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1456304576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1456304576"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Attempts to Solve</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1454559168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -581,6 +1088,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1097,20 +1644,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1124,6 +2187,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1395,268 +2488,506 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B2">
-        <v>6.3899999999999995E-5</v>
-      </c>
-      <c r="C2">
-        <v>3.4299999999999999E-3</v>
-      </c>
-      <c r="D2">
-        <v>0.125</v>
-      </c>
-      <c r="E2">
-        <v>7.5399999999999995E-2</v>
-      </c>
-      <c r="F2">
-        <v>2.3300000000000001E-2</v>
-      </c>
-      <c r="G2">
-        <v>82.8</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.5100000000000002E-4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.4699999999999999E-4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8.76</v>
+      </c>
+      <c r="G2" s="1">
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>1.93E-4</v>
+        <v>3.6900000000000002E-4</v>
       </c>
       <c r="C3">
-        <v>5.6099999999999998E-4</v>
+        <v>4.4799999999999996E-3</v>
       </c>
       <c r="D3">
-        <v>1.3599999999999999E-2</v>
+        <v>4.2200000000000001E-2</v>
       </c>
       <c r="E3">
-        <v>0.4</v>
+        <v>1.59</v>
       </c>
       <c r="F3">
-        <v>7.11</v>
+        <v>9.11</v>
       </c>
       <c r="G3">
-        <v>63.1</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>7.7999999999999999E-5</v>
+        <v>2.4600000000000002E-4</v>
       </c>
       <c r="C4">
-        <v>3.97E-4</v>
+        <v>7.3600000000000002E-3</v>
       </c>
       <c r="D4">
-        <v>9.7000000000000003E-3</v>
+        <v>0.111</v>
       </c>
       <c r="E4">
-        <v>0.94599999999999995</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="F4">
-        <v>25.5</v>
+        <v>1.36</v>
       </c>
       <c r="G4">
-        <v>176</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>5.0899999999999997E-5</v>
+        <v>1.34E-4</v>
       </c>
       <c r="C5">
-        <v>1.3100000000000001E-4</v>
+        <v>2.1800000000000001E-3</v>
       </c>
       <c r="D5">
-        <v>3.2000000000000001E-2</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="E5">
-        <v>0.157</v>
+        <v>0.315</v>
       </c>
       <c r="F5">
-        <v>9.75</v>
+        <v>20.3</v>
       </c>
       <c r="G5">
-        <v>94.5</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>8.4199999999999998E-4</v>
+        <v>1.74E-4</v>
       </c>
       <c r="C6">
-        <v>5.9100000000000003E-3</v>
+        <v>1.56E-3</v>
       </c>
       <c r="D6">
-        <v>8.3899999999999999E-3</v>
+        <v>3.8699999999999998E-2</v>
       </c>
       <c r="E6">
-        <v>1.43E-2</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
-        <v>10.6</v>
+        <v>0.111</v>
       </c>
       <c r="G6">
-        <v>42.9</v>
+        <v>50.9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>2.5999999999999998E-4</v>
+        <v>4.9700000000000005E-4</v>
       </c>
       <c r="C7">
-        <v>7.9100000000000004E-4</v>
+        <v>5.62E-3</v>
       </c>
       <c r="D7">
-        <v>2.46E-2</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="E7">
-        <v>0.54500000000000004</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="F7">
-        <v>1.4</v>
+        <v>22.5</v>
       </c>
       <c r="G7">
-        <v>15.3</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>7.76E-4</v>
+        <v>3.6000000000000001E-5</v>
       </c>
       <c r="C8">
-        <v>6.0599999999999998E-4</v>
+        <v>1.01E-4</v>
       </c>
       <c r="D8">
-        <v>3.6200000000000003E-2</v>
+        <v>6.1199999999999997E-2</v>
       </c>
       <c r="E8">
-        <v>1.3109999999999999</v>
+        <v>4.9500000000000002E-2</v>
       </c>
       <c r="F8">
-        <v>10.5</v>
+        <v>17.7</v>
       </c>
       <c r="G8">
-        <v>148</v>
+        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>2.4699999999999999E-4</v>
+        <v>2.05E-4</v>
       </c>
       <c r="C9">
-        <v>1.57E-3</v>
+        <v>2.2499999999999998E-3</v>
       </c>
       <c r="D9">
-        <v>4.3799999999999999E-2</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E9">
-        <v>3.5000000000000003E-2</v>
+        <v>0.44</v>
       </c>
       <c r="F9">
-        <v>3.64</v>
+        <v>17.5</v>
       </c>
       <c r="G9">
-        <v>98.1</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>4.64E-4</v>
+        <v>1.12E-4</v>
       </c>
       <c r="C10">
-        <v>1.2099999999999999E-3</v>
+        <v>3.5500000000000001E-4</v>
       </c>
       <c r="D10">
-        <v>3.5799999999999998E-2</v>
+        <v>3.49E-2</v>
       </c>
       <c r="E10">
-        <v>0.20799999999999999</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="F10">
-        <v>3.73</v>
+        <v>13</v>
       </c>
       <c r="G10">
-        <v>16</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>1.9599999999999999E-4</v>
+        <v>5.4000000000000001E-4</v>
       </c>
       <c r="C11">
-        <v>6.2600000000000004E-4</v>
+        <v>1.17E-3</v>
       </c>
       <c r="D11">
-        <v>1.2999999999999999E-2</v>
+        <v>1.77E-2</v>
       </c>
       <c r="E11">
-        <v>0.247</v>
+        <v>1.58</v>
       </c>
       <c r="F11">
-        <v>7.86</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="G11">
-        <v>2.71</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <f>AVERAGE(B2:B11)</f>
-        <v>3.1707999999999997E-4</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:H12" si="0">AVERAGE(C2:C11)</f>
-        <v>1.5232000000000002E-3</v>
-      </c>
-      <c r="D12">
+        <v>2.6640000000000002E-4</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
+        <v>2.5323000000000003E-3</v>
+      </c>
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>3.4209000000000003E-2</v>
-      </c>
-      <c r="E12">
+        <v>6.7980000000000013E-2</v>
+      </c>
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0.39387000000000005</v>
-      </c>
-      <c r="F12">
+        <v>0.67805000000000004</v>
+      </c>
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>8.0113299999999992</v>
-      </c>
-      <c r="G12">
+        <v>11.102</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>73.941000000000003</v>
+        <v>202.20000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3490</v>
+      </c>
+      <c r="E13" s="1">
+        <v>61144</v>
+      </c>
+      <c r="F13" s="1">
+        <v>897739</v>
+      </c>
+      <c r="G13" s="1">
+        <v>28053312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>451</v>
+      </c>
+      <c r="D14">
+        <v>3588</v>
+      </c>
+      <c r="E14">
+        <v>136911</v>
+      </c>
+      <c r="F14">
+        <v>878333</v>
+      </c>
+      <c r="G14">
+        <v>37149318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>385</v>
+      </c>
+      <c r="D15">
+        <v>11138</v>
+      </c>
+      <c r="E15">
+        <v>33442</v>
+      </c>
+      <c r="F15">
+        <v>104724</v>
+      </c>
+      <c r="G15">
+        <v>34012516</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>263</v>
+      </c>
+      <c r="D16">
+        <v>3912</v>
+      </c>
+      <c r="E16">
+        <v>18069</v>
+      </c>
+      <c r="F16">
+        <v>1862512</v>
+      </c>
+      <c r="G16">
+        <v>27656127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>185</v>
+      </c>
+      <c r="D17">
+        <v>2972</v>
+      </c>
+      <c r="E17">
+        <v>46235</v>
+      </c>
+      <c r="F17">
+        <v>10279</v>
+      </c>
+      <c r="G17">
+        <v>5129900</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>275</v>
+      </c>
+      <c r="D18">
+        <v>12589</v>
+      </c>
+      <c r="E18">
+        <v>82267</v>
+      </c>
+      <c r="F18">
+        <v>2331717</v>
+      </c>
+      <c r="G18">
+        <v>711417</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>5905</v>
+      </c>
+      <c r="E19">
+        <v>4786</v>
+      </c>
+      <c r="F19">
+        <v>1698956</v>
+      </c>
+      <c r="G19">
+        <v>56269919</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>231</v>
+      </c>
+      <c r="D20">
+        <v>16120</v>
+      </c>
+      <c r="E20">
+        <v>45620</v>
+      </c>
+      <c r="F20">
+        <v>1719680</v>
+      </c>
+      <c r="G20">
+        <v>723567</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <v>3508</v>
+      </c>
+      <c r="E21">
+        <v>38992</v>
+      </c>
+      <c r="F21">
+        <v>1408679</v>
+      </c>
+      <c r="G21">
+        <v>25501191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>61</v>
+      </c>
+      <c r="C22">
+        <v>134</v>
+      </c>
+      <c r="D22">
+        <v>1595</v>
+      </c>
+      <c r="E22">
+        <v>166068</v>
+      </c>
+      <c r="F22">
+        <v>76839</v>
+      </c>
+      <c r="G22">
+        <v>3173367</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <f>AVERAGE(B13:B22)</f>
+        <v>24.3</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" ref="C23:G23" si="1">AVERAGE(C13:C22)</f>
+        <v>200.5</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="1"/>
+        <v>6481.7</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>63353.4</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="1"/>
+        <v>1098945.8</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>21838063.399999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D12:G12 B12:C12" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>